<commit_message>
URLS->HTML-> markdown text -> I use a Gemini LLM model  to cleaning -> markdown file
</commit_message>
<xml_diff>
--- a/scrapy es beautiful soup.xlsx
+++ b/scrapy es beautiful soup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krisztina_PC\flask-chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A15604E8-5905-4339-A5D5-252B2AD5C395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CA91F7-119A-408C-ACCD-44A2BCEDBABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFBAD59B-C419-49C1-949E-F79AE42BD362}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Szempont</t>
   </si>
@@ -135,13 +135,81 @@
   </si>
   <si>
     <t>15.00 MB</t>
+  </si>
+  <si>
+    <t>Adatgyűjtési hatékonyság összehasonlítása (Scrapy vs BeautifulSoup)</t>
+  </si>
+  <si>
+    <r>
+      <t>Scrapy és a BeautifulSoup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> az </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>adatgyűjtés</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> technológiája.</t>
+    </r>
+  </si>
+  <si>
+    <t>Az adatgyűjtési fázis során a Scrapy és a BeautifulSoup könyvtárak teljesítményét hasonlítottam össze különböző URL-ek esetén, mérve a feldolgozási időt,adatgyűjtései sebességet, memóriahasználatot</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A dolgozat célja a Scrapy és a BeautifulSoup könyvtárak összehasonlítása volt az URL-ekből történő adatgyűjtés hatékonysága szempontjából. A vizsgálat során kiderült, hogy bár mindkét eszköz képes strukturált adatok lekérésére, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a HTML elemek manuális feldolgozása jelentős fejlesztői munkát igényel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, különösen eltérő oldalstruktúrák esetén.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +226,22 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="N TIMES ROMAN"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,21 +288,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -553,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6737D196-9BBF-41C1-9B3F-3854051A9D9D}">
-  <dimension ref="B2:H10"/>
+  <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -574,12 +659,12 @@
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="2:8" ht="26.4" customHeight="1">
       <c r="B3" s="2" t="s">
@@ -685,7 +770,7 @@
       <c r="H7" s="2"/>
     </row>
     <row r="10" spans="2:8" ht="69">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D10" t="s">
@@ -693,6 +778,26 @@
       </c>
       <c r="E10" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -705,6 +810,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010098923513FC3A0243A8128825A35AC607" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e8943ab05128516d8cb0e1c3b69cf5db">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a6fef479-ce57-434e-afdf-2ae90e541da3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51a6f781e72d10d33e8da26aa6838af7" ns3:_="">
     <xsd:import namespace="a6fef479-ce57-434e-afdf-2ae90e541da3"/>
@@ -868,22 +988,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A22A89D2-63A3-42E6-8EC3-8310975A492F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a6fef479-ce57-434e-afdf-2ae90e541da3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B77BF88C-08B6-48D8-844C-698466AB92CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3545CCA8-FD8E-45C5-95D7-446FAE4CB8F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -899,28 +1028,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B77BF88C-08B6-48D8-844C-698466AB92CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A22A89D2-63A3-42E6-8EC3-8310975A492F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a6fef479-ce57-434e-afdf-2ae90e541da3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>